<commit_message>
exl data set for home test
</commit_message>
<xml_diff>
--- a/HomePageData.xlsx
+++ b/HomePageData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u6017127\PycharmProjects\SeleniumPython_EndToEnd_Framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F104B8-55D4-4AFA-8102-4CF5847099A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28532077-62B4-47B7-822D-15ACB490342A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6D579D27-90E4-45E4-B615-089E90E85166}"/>
   </bookViews>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Testcase1</t>
   </si>
@@ -44,18 +41,12 @@
     <t>Testcase2</t>
   </si>
   <si>
-    <t xml:space="preserve">email </t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
     <t>gender</t>
   </si>
   <si>
-    <t>Marco</t>
-  </si>
-  <si>
     <t>Gino</t>
   </si>
   <si>
@@ -72,6 +63,12 @@
   </si>
   <si>
     <t>firstname</t>
+  </si>
+  <si>
+    <t>Marco1</t>
+  </si>
+  <si>
+    <t>email</t>
   </si>
 </sst>
 </file>
@@ -437,7 +434,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -447,54 +444,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>12345</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>12345</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>